<commit_message>
fix template excel for example
</commit_message>
<xml_diff>
--- a/dist/Template_Upload_Data_Lisensi.xlsx
+++ b/dist/Template_Upload_Data_Lisensi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/development/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVELOPMENT\PGN\frontend\license-watch-panel\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EED906-FB91-FB41-BC47-EC382F3E39B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99B0319-04B6-4A41-8B13-BE6F7D804183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{DBF3CCF8-1CE0-AA44-ADD7-0E5C9DB1D512}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DBF3CCF8-1CE0-AA44-ADD7-0E5C9DB1D512}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -53,30 +51,6 @@
     <t>North Leone</t>
   </si>
   <si>
-    <t>Zachariah78</t>
-  </si>
-  <si>
-    <t>LcnxlCWSFcwLl00</t>
-  </si>
-  <si>
-    <t>Dooleybury</t>
-  </si>
-  <si>
-    <t>Dedico recusandae spiritus. Sulum cras asper. Rerum adipisci abbas cribro repudiandae cruciamentum quos circumvenio verus.</t>
-  </si>
-  <si>
-    <t>Bryana_OKon37</t>
-  </si>
-  <si>
-    <t>4f4WYVjUgwSJ4Q7</t>
-  </si>
-  <si>
-    <t>South Danny</t>
-  </si>
-  <si>
-    <t>Enim alveus eius auditor creo itaque ipsum. Defaeco una abbas sophismata voro avaritia. Patior vox cibo conforto.</t>
-  </si>
-  <si>
     <t>start_date</t>
   </si>
   <si>
@@ -110,9 +84,6 @@
     <t>Alibaba Cloud</t>
   </si>
   <si>
-    <t>Dell Server</t>
-  </si>
-  <si>
     <t>30/07/2025</t>
   </si>
   <si>
@@ -120,51 +91,6 @@
   </si>
   <si>
     <t>Temptatia una cornu supplanto natus adfero modi velociter. Acsi aggero facere adduco pariatur arbustum. Truculenter accusantium eaque bibo cumque auditor suus ad umquam.</t>
-  </si>
-  <si>
-    <t>Chat GPT4.0</t>
-  </si>
-  <si>
-    <t>Oracle Cloud</t>
-  </si>
-  <si>
-    <t>01/08/2025</t>
-  </si>
-  <si>
-    <t>01/08/2026</t>
-  </si>
-  <si>
-    <t>OracleGuy</t>
-  </si>
-  <si>
-    <t>OraclePass2025</t>
-  </si>
-  <si>
-    <t>East Shania</t>
-  </si>
-  <si>
-    <t>Orci distinctio super. Demum theologus vacuus ulciscor. Vigilo subseco abduco.</t>
-  </si>
-  <si>
-    <t>IBM Cloud</t>
-  </si>
-  <si>
-    <t>10/08/2025</t>
-  </si>
-  <si>
-    <t>10/08/2026</t>
-  </si>
-  <si>
-    <t>ibmuser</t>
-  </si>
-  <si>
-    <t>1bm!Cl0ud</t>
-  </si>
-  <si>
-    <t>Central IBM</t>
-  </si>
-  <si>
-    <t>Cohibeo amplitudo demitto triumphus vinco. Aperio addo viriliter atque dignissimos.</t>
   </si>
 </sst>
 </file>
@@ -228,8 +154,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F796E71F-4686-4042-AA61-A5042EE816A0}" name="Table2" displayName="Table2" ref="A1:K6" totalsRowShown="0">
-  <autoFilter ref="A1:K6" xr:uid="{F796E71F-4686-4042-AA61-A5042EE816A0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F796E71F-4686-4042-AA61-A5042EE816A0}" name="Table2" displayName="Table2" ref="A1:K2" totalsRowShown="0">
+  <autoFilter ref="A1:K2" xr:uid="{F796E71F-4686-4042-AA61-A5042EE816A0}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{734EB893-BB92-EE49-8E13-AA445F7300E0}" name="name"/>
     <tableColumn id="2" xr3:uid="{AAF2BD22-E35E-7A42-919F-CA89EC57ECC5}" name="start_date" dataDxfId="1"/>
@@ -564,13 +490,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45EF172-4301-DE46-AFBA-4995DCD34AC7}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -585,50 +511,50 @@
     <col min="11" max="11" width="146.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D2">
         <v>18</v>
@@ -652,147 +578,7 @@
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>44128</v>
-      </c>
-      <c r="G3">
-        <v>706048</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4">
-        <v>45</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>74707</v>
-      </c>
-      <c r="G4">
-        <v>3361815</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>37200</v>
-      </c>
-      <c r="G5">
-        <v>781200</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>55000</v>
-      </c>
-      <c r="G6">
-        <v>770000</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>